<commit_message>
added results for sex
</commit_message>
<xml_diff>
--- a/Test_results.xlsx
+++ b/Test_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MP\Desktop\1. Projekt\OkCupid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\OneDrive\iTU\First Year Project\OkCupid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CCD9BF-5526-4DB6-BF74-5B894D2A7201}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7ECA258-59A3-474F-988F-C0515D146E6E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13260" yWindow="900" windowWidth="17280" windowHeight="8964" xr2:uid="{DEDE9B50-EA2C-41DA-A9FF-A2715E97E0A1}"/>
+    <workbookView xWindow="435" yWindow="495" windowWidth="9570" windowHeight="10440" xr2:uid="{DEDE9B50-EA2C-41DA-A9FF-A2715E97E0A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="25">
   <si>
     <t>Okcupid.py</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>0.68</t>
+  </si>
+  <si>
+    <t>Sex</t>
   </si>
 </sst>
 </file>
@@ -236,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -244,6 +247,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -262,7 +266,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -558,22 +562,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F4F48E-6CBD-423D-AA91-5FF20D8C2A31}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -590,7 +594,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -607,7 +611,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -624,7 +628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -641,7 +645,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -658,7 +662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -675,7 +679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -692,7 +696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -709,7 +713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -726,7 +730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -743,7 +747,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -760,7 +764,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -777,7 +781,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
@@ -794,7 +798,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -811,7 +815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -828,7 +832,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -845,7 +849,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -860,6 +864,74 @@
       </c>
       <c r="E17" s="6" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.59</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated okcupid.py with function to binarize labels
</commit_message>
<xml_diff>
--- a/Test_results.xlsx
+++ b/Test_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OkCupid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5079028-18D7-4B33-AF58-29A499B98083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4019CF8-32D0-4BFF-B360-17ED7C8FD6E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DEDE9B50-EA2C-41DA-A9FF-A2715E97E0A1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="158">
   <si>
     <t>Okcupid.py</t>
   </si>
@@ -478,6 +478,33 @@
   </si>
   <si>
     <t>essay4 bigram sex</t>
+  </si>
+  <si>
+    <t>essay0 essay0 words</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>unigram</t>
+  </si>
+  <si>
+    <t>essay0 essay0 bigrams</t>
+  </si>
+  <si>
+    <t>bigram</t>
+  </si>
+  <si>
+    <t>f F1-Score: 0.5337704918032787</t>
+  </si>
+  <si>
+    <t>m F1-Score: 0.6310326933056565</t>
+  </si>
+  <si>
+    <t>trigram</t>
+  </si>
+  <si>
+    <t>essay 4</t>
   </si>
 </sst>
 </file>
@@ -796,14 +823,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>61451</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>385206</xdr:colOff>
-      <xdr:row>108</xdr:row>
-      <xdr:rowOff>181310</xdr:rowOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>181311</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1136,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F4F48E-6CBD-423D-AA91-5FF20D8C2A31}">
-  <dimension ref="A1:S101"/>
+  <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="93" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView tabSelected="1" topLeftCell="B85" zoomScale="93" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I115" sqref="I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3449,40 +3476,95 @@
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="B100" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F100" s="1">
+        <v>62.1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E101" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F102" s="1">
+        <v>58.8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E103" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F100" s="1">
+      <c r="D105" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F105" s="1">
         <v>66.8</v>
       </c>
-      <c r="J100" t="s">
+      <c r="J105" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B101" s="1" t="s">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F101" s="1">
+      <c r="D106" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F106" s="1">
         <v>64.62</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B107" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F107" s="1">
+        <v>57.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>